<commit_message>
Calculate T6 enzyme activity
Last time I left off at processing T6 dry weights. I used the process T6 dry weights to calculate T6 enzyme activity. Now, I'm looking at each figure in each time point for both hydrolytic & oxidative enzymes to see whether there is noisy or otherwise bad data. Steve suggested that the noisy data is due to low enzyme activity.
</commit_message>
<xml_diff>
--- a/Unprocessed activity graphs/Samples with errors.xlsx
+++ b/Unprocessed activity graphs/Samples with errors.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Documents\UCI undergrad\Bio-ESS 199\Microbial enzyme activity in leaf litter\Unprocessed activity graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91ADCAA-97A9-4D46-BE8D-C35CD053DBD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6351DA-CB92-4941-8407-746755E62CD2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F0624B8F-E787-4348-B519-0FF9F7B802E3}"/>
   </bookViews>
   <sheets>
     <sheet name="T0" sheetId="1" r:id="rId1"/>
     <sheet name="T3" sheetId="3" r:id="rId2"/>
+    <sheet name="T5" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="34">
   <si>
     <t>4LXX</t>
   </si>
@@ -112,13 +113,31 @@
     <t>x</t>
   </si>
   <si>
-    <t>Any x's mark bad enzymes for a particular sample that need a redo. Any o's signify substrate inhibition. Any a's mark that the enzyme is salvageable with other errors</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>o = possible substrate inhibition</t>
+  </si>
+  <si>
+    <t>a = salvageable with other errors</t>
+  </si>
+  <si>
+    <t>x = noisy, indicating low activity or bad data</t>
+  </si>
+  <si>
+    <t>PPO</t>
+  </si>
+  <si>
+    <t>PER</t>
+  </si>
+  <si>
+    <t>y = generally negative activity, indicating no activity or need to improve methodology</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -494,17 +513,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9579520-90FA-4D77-9373-A89FBEFF1BF4}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H21"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>16</v>
@@ -527,16 +546,31 @@
       <c r="H1" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -549,8 +583,17 @@
       <c r="H3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -560,8 +603,17 @@
       <c r="H4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -574,8 +626,17 @@
       <c r="H5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -585,8 +646,14 @@
       <c r="H6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -599,24 +666,36 @@
       <c r="H7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -635,16 +714,28 @@
       <c r="H10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -660,13 +751,19 @@
       <c r="H12" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
         <v>23</v>
@@ -677,8 +774,11 @@
       <c r="H13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -688,8 +788,14 @@
       <c r="H14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -703,15 +809,21 @@
         <v>24</v>
       </c>
       <c r="H15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="I15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
@@ -731,8 +843,14 @@
       <c r="H16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -748,10 +866,8 @@
       <c r="H17" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>25</v>
+      <c r="J17" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -762,17 +878,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB4ECC9-B3D0-4C1F-A134-260A7669F713}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>16</v>
@@ -795,8 +911,14 @@
       <c r="H1" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -812,8 +934,11 @@
       <c r="H2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -826,13 +951,19 @@
       <c r="H3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -842,8 +973,11 @@
       <c r="D5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -857,7 +991,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -868,7 +1002,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -882,7 +1016,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -893,7 +1027,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -904,7 +1038,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -912,7 +1046,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -920,7 +1054,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -931,7 +1065,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -942,12 +1076,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -963,12 +1097,19 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30D1CA8-4626-4EB5-8FAC-20B4A65BCE9B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Judging T5 enzyme data
I classified error types in the T5 data after looking at the graphs of enzyme activity. I judged the graphs to see if the data looks noisy or not, if there is any signs of substrate inhibition, or, in the case of peroxidase, if there is a decreasing trend in enzyme activity as substrate concentration increases.

Steve previously suggested that if the data looks especially noisy, then that that's a sign of low enzyme activity, so low that the plate reader only picked up noise. So I'm going with that suggestion for now. So, when I see noisy data, it generally makes me believe that there is low enzyme activity.
</commit_message>
<xml_diff>
--- a/Unprocessed activity graphs/Samples with errors.xlsx
+++ b/Unprocessed activity graphs/Samples with errors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Documents\UCI undergrad\Bio-ESS 199\Microbial enzyme activity in leaf litter\Unprocessed activity graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6351DA-CB92-4941-8407-746755E62CD2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF5A573-89E3-4FA2-AF1D-F9E0E2144088}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F0624B8F-E787-4348-B519-0FF9F7B802E3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{F0624B8F-E787-4348-B519-0FF9F7B802E3}"/>
   </bookViews>
   <sheets>
     <sheet name="T0" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="34">
   <si>
     <t>4LXX</t>
   </si>
@@ -516,7 +516,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -705,14 +705,8 @@
       <c r="D10" t="s">
         <v>23</v>
       </c>
-      <c r="F10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" t="s">
-        <v>23</v>
-      </c>
       <c r="H10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I10" t="s">
         <v>25</v>
@@ -880,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB4ECC9-B3D0-4C1F-A134-260A7669F713}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -934,6 +928,9 @@
       <c r="H2" t="s">
         <v>23</v>
       </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
       <c r="K2" t="s">
         <v>29</v>
       </c>
@@ -951,6 +948,9 @@
       <c r="H3" t="s">
         <v>23</v>
       </c>
+      <c r="J3" t="s">
+        <v>33</v>
+      </c>
       <c r="K3" t="s">
         <v>27</v>
       </c>
@@ -959,6 +959,12 @@
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>33</v>
+      </c>
       <c r="K4" t="s">
         <v>28</v>
       </c>
@@ -973,6 +979,9 @@
       <c r="D5" t="s">
         <v>23</v>
       </c>
+      <c r="J5" t="s">
+        <v>33</v>
+      </c>
       <c r="K5" t="s">
         <v>32</v>
       </c>
@@ -990,6 +999,9 @@
       <c r="H6" t="s">
         <v>23</v>
       </c>
+      <c r="J6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -1001,6 +1013,9 @@
       <c r="H7" t="s">
         <v>23</v>
       </c>
+      <c r="J7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -1015,6 +1030,12 @@
       <c r="H8" t="s">
         <v>23</v>
       </c>
+      <c r="I8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -1026,6 +1047,12 @@
       <c r="H9" t="s">
         <v>23</v>
       </c>
+      <c r="I9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -1037,6 +1064,12 @@
       <c r="H10" t="s">
         <v>23</v>
       </c>
+      <c r="I10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -1045,6 +1078,12 @@
       <c r="H11" t="s">
         <v>23</v>
       </c>
+      <c r="I11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -1053,6 +1092,12 @@
       <c r="H12" t="s">
         <v>23</v>
       </c>
+      <c r="I12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -1064,6 +1109,12 @@
       <c r="H13" t="s">
         <v>23</v>
       </c>
+      <c r="I13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
@@ -1075,18 +1126,33 @@
       <c r="H14" t="s">
         <v>23</v>
       </c>
+      <c r="I14" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="J15" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1095,6 +1161,12 @@
       </c>
       <c r="G17" t="s">
         <v>24</v>
+      </c>
+      <c r="I17" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1104,12 +1176,328 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30D1CA8-4626-4EB5-8FAC-20B4A65BCE9B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished annotating errors in data qc, outputting calculated enzyme activity
So yeah, I finished looking through the raw enzyme activity graphs of all time points and I noted down the types of "errors" present in them for me to do further quality control. To restate, I'm judging whether a sample's enzyme is experiencing substrate inhibition, shows very noisy activity, negative activity in general, or have a few data points of negative activity that are still salvageable.

I also outputted the calculated enzyme activity values. I'm going to write a new script to do some further processing of the calculated enzyme activity values rather than the raw data. I already made the script, and I'll continue working on the script.
</commit_message>
<xml_diff>
--- a/Unprocessed activity graphs/Samples with errors.xlsx
+++ b/Unprocessed activity graphs/Samples with errors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Documents\UCI undergrad\Bio-ESS 199\Microbial enzyme activity in leaf litter\Unprocessed activity graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF5A573-89E3-4FA2-AF1D-F9E0E2144088}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1987CD14-3B00-4B91-A6AA-4DB62A818D42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{F0624B8F-E787-4348-B519-0FF9F7B802E3}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="T0" sheetId="1" r:id="rId1"/>
     <sheet name="T3" sheetId="3" r:id="rId2"/>
     <sheet name="T5" sheetId="4" r:id="rId3"/>
+    <sheet name="T6" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="38">
   <si>
     <t>4LXX</t>
   </si>
@@ -128,16 +129,28 @@
     <t>x = noisy, indicating low activity or bad data</t>
   </si>
   <si>
-    <t>PPO</t>
-  </si>
-  <si>
-    <t>PER</t>
-  </si>
-  <si>
     <t>y = generally negative activity, indicating no activity or need to improve methodology</t>
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>PPO rep 2</t>
+  </si>
+  <si>
+    <t>PER rep 2</t>
+  </si>
+  <si>
+    <t>PPO rep 1</t>
+  </si>
+  <si>
+    <t>PER rep 1</t>
+  </si>
+  <si>
+    <t>PPO rep 3</t>
+  </si>
+  <si>
+    <t>PPO rep 4</t>
   </si>
 </sst>
 </file>
@@ -513,15 +526,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9579520-90FA-4D77-9373-A89FBEFF1BF4}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
@@ -547,13 +560,19 @@
         <v>22</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -564,13 +583,19 @@
         <v>25</v>
       </c>
       <c r="J2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -586,14 +611,17 @@
       <c r="I3" t="s">
         <v>25</v>
       </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
       <c r="K3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -603,17 +631,20 @@
       <c r="H4" t="s">
         <v>23</v>
       </c>
-      <c r="I4" t="s">
-        <v>25</v>
-      </c>
       <c r="J4" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="K4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -626,17 +657,20 @@
       <c r="H5" t="s">
         <v>23</v>
       </c>
-      <c r="I5" t="s">
-        <v>25</v>
-      </c>
       <c r="J5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="L5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -650,10 +684,16 @@
         <v>25</v>
       </c>
       <c r="J6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="K6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -666,36 +706,45 @@
       <c r="H7" t="s">
         <v>23</v>
       </c>
-      <c r="I7" t="s">
-        <v>25</v>
-      </c>
       <c r="J7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="K7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G8" t="s">
         <v>23</v>
       </c>
-      <c r="J8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D9" t="s">
         <v>23</v>
       </c>
-      <c r="J9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -712,10 +761,16 @@
         <v>25</v>
       </c>
       <c r="J10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="K10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -726,10 +781,16 @@
         <v>25</v>
       </c>
       <c r="J11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="K11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -749,10 +810,16 @@
         <v>25</v>
       </c>
       <c r="J12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="K12" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -768,11 +835,14 @@
       <c r="H13" t="s">
         <v>23</v>
       </c>
-      <c r="J13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K13" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -782,14 +852,17 @@
       <c r="H14" t="s">
         <v>23</v>
       </c>
-      <c r="I14" t="s">
-        <v>25</v>
-      </c>
       <c r="J14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="K14" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -808,11 +881,14 @@
       <c r="I15" t="s">
         <v>25</v>
       </c>
-      <c r="J15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K15" t="s">
+        <v>31</v>
+      </c>
+      <c r="L15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -841,10 +917,16 @@
         <v>25</v>
       </c>
       <c r="J16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="K16" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -860,8 +942,11 @@
       <c r="H17" t="s">
         <v>23</v>
       </c>
-      <c r="J17" t="s">
-        <v>33</v>
+      <c r="K17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L17" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -872,15 +957,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB4ECC9-B3D0-4C1F-A134-260A7669F713}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
@@ -906,13 +991,19 @@
         <v>22</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -928,14 +1019,17 @@
       <c r="H2" t="s">
         <v>23</v>
       </c>
-      <c r="J2" t="s">
-        <v>33</v>
-      </c>
       <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -948,28 +1042,34 @@
       <c r="H3" t="s">
         <v>23</v>
       </c>
-      <c r="J3" t="s">
-        <v>33</v>
-      </c>
       <c r="K3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I4" t="s">
         <v>25</v>
       </c>
-      <c r="J4" t="s">
-        <v>33</v>
-      </c>
       <c r="K4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -979,14 +1079,17 @@
       <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="J5" t="s">
-        <v>33</v>
-      </c>
       <c r="K5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="L5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -999,11 +1102,14 @@
       <c r="H6" t="s">
         <v>23</v>
       </c>
-      <c r="J6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1013,11 +1119,20 @@
       <c r="H7" t="s">
         <v>23</v>
       </c>
+      <c r="I7" t="s">
+        <v>25</v>
+      </c>
       <c r="J7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="K7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1034,10 +1149,16 @@
         <v>25</v>
       </c>
       <c r="J8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="K8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -1051,10 +1172,16 @@
         <v>24</v>
       </c>
       <c r="J9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="K9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1068,10 +1195,16 @@
         <v>24</v>
       </c>
       <c r="J10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="K10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1082,10 +1215,16 @@
         <v>25</v>
       </c>
       <c r="J11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="K11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1096,10 +1235,16 @@
         <v>25</v>
       </c>
       <c r="J12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="K12" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1113,10 +1258,16 @@
         <v>25</v>
       </c>
       <c r="J13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="K13" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1130,18 +1281,24 @@
         <v>24</v>
       </c>
       <c r="J14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="K14" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="L15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1151,8 +1308,14 @@
       <c r="J16" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K16" t="s">
+        <v>24</v>
+      </c>
+      <c r="L16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1166,7 +1329,13 @@
         <v>24</v>
       </c>
       <c r="J17" t="s">
-        <v>33</v>
+        <v>23</v>
+      </c>
+      <c r="K17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L17" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1176,15 +1345,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30D1CA8-4626-4EB5-8FAC-20B4A65BCE9B}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
@@ -1210,13 +1379,32 @@
         <v>22</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1239,13 +1427,19 @@
         <v>25</v>
       </c>
       <c r="J2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1256,13 +1450,19 @@
         <v>25</v>
       </c>
       <c r="J3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1272,14 +1472,17 @@
       <c r="H4" t="s">
         <v>23</v>
       </c>
-      <c r="J4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1290,13 +1493,19 @@
         <v>25</v>
       </c>
       <c r="J5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="M5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1306,14 +1515,17 @@
       <c r="H6" t="s">
         <v>23</v>
       </c>
-      <c r="I6" t="s">
-        <v>25</v>
-      </c>
       <c r="J6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="M6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1336,35 +1548,44 @@
         <v>25</v>
       </c>
       <c r="J7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="M7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H8" t="s">
         <v>23</v>
       </c>
-      <c r="I8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M8" t="s">
+        <v>31</v>
+      </c>
+      <c r="N8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I9" t="s">
-        <v>25</v>
-      </c>
       <c r="J9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1383,11 +1604,14 @@
       <c r="I10" t="s">
         <v>25</v>
       </c>
-      <c r="J10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1401,10 +1625,16 @@
         <v>25</v>
       </c>
       <c r="J11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="M11" t="s">
+        <v>31</v>
+      </c>
+      <c r="N11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1420,11 +1650,14 @@
       <c r="I12" t="s">
         <v>25</v>
       </c>
-      <c r="J12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1432,10 +1665,16 @@
         <v>25</v>
       </c>
       <c r="J13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="M13" t="s">
+        <v>31</v>
+      </c>
+      <c r="N13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1446,13 +1685,16 @@
         <v>23</v>
       </c>
       <c r="I14" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="M14" t="s">
+        <v>24</v>
+      </c>
+      <c r="N14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -1468,8 +1710,17 @@
       <c r="H15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" t="s">
+        <v>31</v>
+      </c>
+      <c r="N15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1479,8 +1730,29 @@
       <c r="H16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L16" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N16" t="s">
+        <v>31</v>
+      </c>
+      <c r="O16" t="s">
+        <v>31</v>
+      </c>
+      <c r="P16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1495,6 +1767,431 @@
       </c>
       <c r="H17" t="s">
         <v>23</v>
+      </c>
+      <c r="M17" t="s">
+        <v>31</v>
+      </c>
+      <c r="N17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58CC1B67-993C-44F0-B51A-D0BFAF9267BE}">
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" t="s">
+        <v>31</v>
+      </c>
+      <c r="L15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L17" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Obtained parameters up to T5 oxidase
Sample 47RRX is giving me trouble for T5 oxidase. I'm still trying to obtain the parameters for this dataset, I haven't even plotted the actual and predicted enzyme activities yet. But, I'm done obtaining parameters & plotting actual & predicted activities for the previous time points and also T5 hydrolase.
</commit_message>
<xml_diff>
--- a/Unprocessed activity graphs/Samples with errors.xlsx
+++ b/Unprocessed activity graphs/Samples with errors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Documents\UCI undergrad\Bio-ESS 199\Microbial enzyme activity in leaf litter\Unprocessed activity graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E03DAEC-848F-4002-8A7E-AF4DA9A0E9B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8736F2D-01EF-48E4-8BD1-9B63690639FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F0624B8F-E787-4348-B519-0FF9F7B802E3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{F0624B8F-E787-4348-B519-0FF9F7B802E3}"/>
   </bookViews>
   <sheets>
     <sheet name="T0" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="38">
   <si>
     <t>4LXX</t>
   </si>
@@ -977,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB4ECC9-B3D0-4C1F-A134-260A7669F713}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1028,9 +1028,6 @@
       <c r="C2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
       <c r="H2" t="s">
         <v>23</v>
       </c>
@@ -1114,9 +1111,6 @@
       <c r="E6" t="s">
         <v>23</v>
       </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
       <c r="K6" t="s">
         <v>31</v>
       </c>
@@ -1157,9 +1151,6 @@
       <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
       <c r="H8" t="s">
         <v>23</v>
       </c>
@@ -1207,9 +1198,6 @@
         <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" t="s">
         <v>23</v>
       </c>
       <c r="I10" t="s">
@@ -1360,7 +1348,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1524,9 +1512,6 @@
       <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
       <c r="J6" t="s">
         <v>25</v>
       </c>
@@ -1541,9 +1526,6 @@
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
       <c r="C7" t="s">
         <v>23</v>
       </c>
@@ -1551,6 +1533,9 @@
         <v>23</v>
       </c>
       <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
         <v>23</v>
       </c>
       <c r="H7" t="s">
@@ -1608,7 +1593,7 @@
         <v>23</v>
       </c>
       <c r="G10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H10" t="s">
         <v>23</v>
@@ -1654,7 +1639,7 @@
         <v>25</v>
       </c>
       <c r="G12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H12" t="s">
         <v>23</v>
@@ -1673,6 +1658,9 @@
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="H13" t="s">
+        <v>23</v>
+      </c>
       <c r="I13" t="s">
         <v>25</v>
       </c>
@@ -1714,7 +1702,7 @@
         <v>24</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F15" t="s">
         <v>23</v>
@@ -1796,8 +1784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58CC1B67-993C-44F0-B51A-D0BFAF9267BE}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Obtained T6 parameters and exported parameters and cleaned activity data as new Excel files
I cleaned and obtained T6 parameters as well as graphed T6 activity. With that done, I have obtained parameters for all time points as well as cleaned all enzyme activity. Hooray!

I exported the cleaned enzyme activity and parameter values as separate Excel files. Now, time to start doing statistical analyses.
</commit_message>
<xml_diff>
--- a/Unprocessed activity graphs/Samples with errors.xlsx
+++ b/Unprocessed activity graphs/Samples with errors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Documents\UCI undergrad\Bio-ESS 199\Microbial enzyme activity in leaf litter\Unprocessed activity graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8736F2D-01EF-48E4-8BD1-9B63690639FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D34086D-8BAD-4A4C-A670-3591966295A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{F0624B8F-E787-4348-B519-0FF9F7B802E3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="38">
   <si>
     <t>4LXX</t>
   </si>
@@ -1785,7 +1785,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1946,9 +1946,6 @@
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
       <c r="H6" t="s">
         <v>23</v>
       </c>
@@ -1995,9 +1992,6 @@
       <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="H8" t="s">
-        <v>23</v>
-      </c>
       <c r="I8" t="s">
         <v>25</v>
       </c>
@@ -2176,7 +2170,7 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" t="s">
         <v>23</v>

</xml_diff>